<commit_message>
WIP MDT demo Jan Willem
</commit_message>
<xml_diff>
--- a/MDT/RollenEnBeheerdersPassen/RdwDienst.xlsx
+++ b/MDT/RollenEnBeheerdersPassen/RdwDienst.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="16272" windowHeight="12072"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="16272" windowHeight="12072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RDWDiensten" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
+    <sheet name="Mailtje" sheetId="2" r:id="rId2"/>
+    <sheet name="nodigVoor" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
   <si>
     <t>1. Vrijwaren</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>[ProcIdent;]</t>
+  </si>
+  <si>
+    <t>ProcIdent</t>
+  </si>
+  <si>
+    <t>[nodigVoor]</t>
   </si>
 </sst>
 </file>
@@ -513,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -527,6 +533,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -833,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,7 +977,7 @@
   <dimension ref="B3:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B37"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,12 +1144,552 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="5">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="5">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="5">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="5">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="5">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="5">
+        <v>2842</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="5">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="5">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="5">
+        <v>2868</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="5">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="5">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="5">
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="5">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="5">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="5">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="5">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2547</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="5">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="5">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="5">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="5">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="5">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="5">
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="5">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="5">
+        <v>2726</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="5">
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="5">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="5">
+        <v>2747</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64" s="5">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="5">
+        <v>2959</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="5">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="5">
+        <v>3050</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP MDT Diensten voor VN van Jan Willem toegepast
</commit_message>
<xml_diff>
--- a/MDT/RollenEnBeheerdersPassen/RdwDienst.xlsx
+++ b/MDT/RollenEnBeheerdersPassen/RdwDienst.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>1. Vrijwaren</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>[nodigVoor]</t>
+  </si>
+  <si>
+    <t>nodigVoor</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -515,11 +518,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -534,6 +552,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1146,11 +1166,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1158,536 +1180,331 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="5">
-        <v>237</v>
+      <c r="A3" s="6">
+        <v>1115</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="5">
-        <v>364</v>
+      <c r="A4" s="6">
+        <v>1116</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="5">
-        <v>365</v>
+      <c r="A5" s="6">
+        <v>1117</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="5">
-        <v>366</v>
+      <c r="A6" s="6">
+        <v>1302</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="5">
-        <v>521</v>
+      <c r="A7" s="6">
+        <v>1869</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="5">
-        <v>658</v>
+      <c r="A8" s="6">
+        <v>2628</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="5">
-        <v>731</v>
+      <c r="A9" s="6">
+        <v>2629</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="5">
-        <v>734</v>
+      <c r="A10" s="6">
+        <v>2630</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1023</v>
+      <c r="A11" s="6">
+        <v>2631</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1033</v>
+      <c r="A12" s="6">
+        <v>2632</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1114</v>
+      <c r="A13" s="6">
+        <v>2693</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1122</v>
+      <c r="A14" s="6">
+        <v>2797</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="5">
-        <v>1426</v>
+      <c r="A15" s="6">
+        <v>2798</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1433</v>
+      <c r="A16" s="6">
+        <v>2800</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="5">
-        <v>1440</v>
+      <c r="A17" s="6">
+        <v>2801</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1447</v>
+      <c r="A18" s="6">
+        <v>2802</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="5">
-        <v>1544</v>
+      <c r="A19" s="6">
+        <v>2803</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1573</v>
+      <c r="A20" s="6">
+        <v>2804</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1574</v>
+      <c r="A21" s="6">
+        <v>2809</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1575</v>
+      <c r="A22" s="6">
+        <v>2876</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="5">
-        <v>1576</v>
+      <c r="A23" s="6">
+        <v>2878</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="5">
-        <v>2056</v>
+      <c r="A24" s="6">
+        <v>2879</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="5">
-        <v>2086</v>
+      <c r="A25" s="6">
+        <v>3059</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="5">
-        <v>2159</v>
+      <c r="A26" s="6">
+        <v>695</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="5">
-        <v>2174</v>
-      </c>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="5">
-        <v>2259</v>
-      </c>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="5">
-        <v>2273</v>
-      </c>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="5">
-        <v>2298</v>
-      </c>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="5">
-        <v>2390</v>
-      </c>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="5">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="5">
-        <v>2502</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="5">
-        <v>2632</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="5">
-        <v>2803</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="5">
-        <v>2842</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="5">
-        <v>2847</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="5">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="5">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="5">
-        <v>2866</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="5">
-        <v>2868</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="5">
-        <v>2869</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="5">
-        <v>2882</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="5">
-        <v>2884</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="5">
-        <v>2983</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5">
-        <v>3018</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="5">
-        <v>3048</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="5">
-        <v>3059</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="5">
-        <v>3070</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="5">
-        <v>3073</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="5">
-        <v>2547</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53" s="5">
-        <v>2548</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="5">
-        <v>2609</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>44</v>
-      </c>
-      <c r="B55" s="5">
-        <v>2625</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>44</v>
-      </c>
-      <c r="B56" s="5">
-        <v>2626</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="5">
-        <v>2627</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58" s="5">
-        <v>2697</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>44</v>
-      </c>
-      <c r="B59" s="5">
-        <v>2701</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="5">
-        <v>2726</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>44</v>
-      </c>
-      <c r="B61" s="5">
-        <v>2727</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" s="5">
-        <v>2745</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="5">
-        <v>2747</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="5">
-        <v>2760</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>44</v>
-      </c>
-      <c r="B65" s="5">
-        <v>2902</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>44</v>
-      </c>
-      <c r="B66" s="5">
-        <v>2959</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>44</v>
-      </c>
-      <c r="B67" s="5">
-        <v>2967</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>44</v>
-      </c>
-      <c r="B68" s="5">
-        <v>3050</v>
-      </c>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="5"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="5"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>